<commit_message>
Refactor UnitSchema to update sub_specialty_id field name
</commit_message>
<xml_diff>
--- a/data/test_data_masterplan.xlsx
+++ b/data/test_data_masterplan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\visual_mandiri_informatika\surgery\backend_surgery_fastapi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\visual_mandiri_informatika\surgery\backend_surgery_fastapi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0D5A73-8839-49BE-A039-B82BEACD084B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F967C4-C316-489F-9F25-EFB88402918B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1328,7 +1328,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="2">
-        <v>45546</v>
+        <v>45551</v>
       </c>
       <c r="B2" s="2">
         <v>44929</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="2">
-        <v>45545</v>
+        <v>45552</v>
       </c>
       <c r="B3" s="2">
         <v>44930</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="2">
-        <v>44861</v>
+        <v>45553</v>
       </c>
       <c r="B4" s="2">
         <v>44929</v>

</xml_diff>

<commit_message>
fix generate master plan => (AI OT Manager Testing II (20241106))
</commit_message>
<xml_diff>
--- a/data/test_data_masterplan.xlsx
+++ b/data/test_data_masterplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\visual_mandiri_informatika\surgery\backend_surgery_fastapi\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rizfan\Documents\project\vmi\surgery\backend_surgery_fastapi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3146B73F-5A4F-4989-BC05-4D5035A3FC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC15F9F-4CD9-4AA2-AC4F-B65852BBF705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1329,9 +1329,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
check clashing in ot
</commit_message>
<xml_diff>
--- a/data/test_data_masterplan.xlsx
+++ b/data/test_data_masterplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rizfan\Documents\project\vmi\surgery\backend_surgery_fastapi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17DA799-733F-4332-8AE2-511D047D5703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB8C29C-D0D4-4516-974F-3FDA5F977C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="285">
   <si>
     <t>AGE</t>
   </si>
@@ -1327,11 +1327,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52:XFD66"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1447,7 +1447,7 @@
         <v>24</v>
       </c>
       <c r="M2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="N2" t="s">
         <v>25</v>
@@ -1500,7 +1500,7 @@
         <v>34</v>
       </c>
       <c r="M3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N3" t="s">
         <v>35</v>
@@ -1553,7 +1553,7 @@
         <v>24</v>
       </c>
       <c r="M4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N4" t="s">
         <v>42</v>
@@ -1606,7 +1606,7 @@
         <v>24</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N5" t="s">
         <v>48</v>
@@ -1659,7 +1659,7 @@
         <v>55</v>
       </c>
       <c r="M6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N6" t="s">
         <v>56</v>
@@ -1712,7 +1712,7 @@
         <v>24</v>
       </c>
       <c r="M7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N7" t="s">
         <v>63</v>
@@ -1818,7 +1818,7 @@
         <v>24</v>
       </c>
       <c r="M9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N9" t="s">
         <v>77</v>
@@ -1871,7 +1871,7 @@
         <v>83</v>
       </c>
       <c r="M10">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N10" t="s">
         <v>84</v>
@@ -1924,7 +1924,7 @@
         <v>91</v>
       </c>
       <c r="M11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N11" t="s">
         <v>92</v>
@@ -1977,7 +1977,7 @@
         <v>90</v>
       </c>
       <c r="M12">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="N12" t="s">
         <v>97</v>
@@ -2027,7 +2027,7 @@
         <v>34</v>
       </c>
       <c r="M13">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="N13" t="s">
         <v>71</v>
@@ -2080,7 +2080,7 @@
         <v>34</v>
       </c>
       <c r="M14">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="N14" t="s">
         <v>106</v>
@@ -2133,7 +2133,7 @@
         <v>24</v>
       </c>
       <c r="M15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N15" t="s">
         <v>84</v>
@@ -2186,7 +2186,7 @@
         <v>24</v>
       </c>
       <c r="M16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N16" t="s">
         <v>114</v>
@@ -2239,7 +2239,7 @@
         <v>24</v>
       </c>
       <c r="M17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N17" t="s">
         <v>118</v>
@@ -2292,7 +2292,7 @@
         <v>91</v>
       </c>
       <c r="M18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N18" t="s">
         <v>124</v>
@@ -2345,7 +2345,7 @@
         <v>24</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N19" t="s">
         <v>129</v>
@@ -2398,7 +2398,7 @@
         <v>24</v>
       </c>
       <c r="M20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N20" t="s">
         <v>133</v>
@@ -2451,7 +2451,7 @@
         <v>91</v>
       </c>
       <c r="M21">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="N21" t="s">
         <v>25</v>
@@ -2504,7 +2504,7 @@
         <v>24</v>
       </c>
       <c r="M22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N22" t="s">
         <v>124</v>
@@ -2557,7 +2557,7 @@
         <v>24</v>
       </c>
       <c r="M23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N23" t="s">
         <v>144</v>
@@ -2663,7 +2663,7 @@
         <v>91</v>
       </c>
       <c r="M25">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="N25" t="s">
         <v>157</v>
@@ -2713,7 +2713,7 @@
         <v>55</v>
       </c>
       <c r="M26">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="N26" t="s">
         <v>63</v>
@@ -2763,7 +2763,7 @@
         <v>55</v>
       </c>
       <c r="M27">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="N27" t="s">
         <v>77</v>
@@ -2816,7 +2816,7 @@
         <v>91</v>
       </c>
       <c r="M28">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N28" t="s">
         <v>118</v>
@@ -2869,7 +2869,7 @@
         <v>83</v>
       </c>
       <c r="M29">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="N29" t="s">
         <v>133</v>
@@ -2922,7 +2922,7 @@
         <v>90</v>
       </c>
       <c r="M30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N30" t="s">
         <v>144</v>
@@ -2975,7 +2975,7 @@
         <v>34</v>
       </c>
       <c r="M31">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N31" t="s">
         <v>183</v>
@@ -3081,7 +3081,7 @@
         <v>90</v>
       </c>
       <c r="M33">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N33" t="s">
         <v>196</v>
@@ -3134,7 +3134,7 @@
         <v>90</v>
       </c>
       <c r="M34">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N34" t="s">
         <v>97</v>
@@ -3187,7 +3187,7 @@
         <v>24</v>
       </c>
       <c r="M35">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="N35" t="s">
         <v>201</v>
@@ -3240,7 +3240,7 @@
         <v>90</v>
       </c>
       <c r="M36">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N36" t="s">
         <v>205</v>
@@ -3293,7 +3293,7 @@
         <v>24</v>
       </c>
       <c r="M37">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N37" t="s">
         <v>201</v>
@@ -3346,7 +3346,7 @@
         <v>216</v>
       </c>
       <c r="M38">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N38" t="s">
         <v>189</v>
@@ -3399,7 +3399,7 @@
         <v>91</v>
       </c>
       <c r="M39">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="N39" t="s">
         <v>183</v>
@@ -3505,7 +3505,7 @@
         <v>83</v>
       </c>
       <c r="M41">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N41" t="s">
         <v>129</v>
@@ -3558,7 +3558,7 @@
         <v>90</v>
       </c>
       <c r="M42">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="N42" t="s">
         <v>205</v>
@@ -3611,7 +3611,7 @@
         <v>90</v>
       </c>
       <c r="M43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N43" t="s">
         <v>92</v>
@@ -3664,7 +3664,7 @@
         <v>91</v>
       </c>
       <c r="M44">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N44" t="s">
         <v>196</v>
@@ -3717,7 +3717,7 @@
         <v>34</v>
       </c>
       <c r="M45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N45" t="s">
         <v>35</v>
@@ -3770,7 +3770,7 @@
         <v>91</v>
       </c>
       <c r="M46">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="N46" t="s">
         <v>230</v>
@@ -3823,7 +3823,7 @@
         <v>34</v>
       </c>
       <c r="M47">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="N47" t="s">
         <v>106</v>
@@ -3876,7 +3876,7 @@
         <v>34</v>
       </c>
       <c r="M48">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N48" t="s">
         <v>42</v>
@@ -3929,7 +3929,7 @@
         <v>83</v>
       </c>
       <c r="M49">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N49" t="s">
         <v>48</v>
@@ -3982,7 +3982,7 @@
         <v>34</v>
       </c>
       <c r="M50">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N50" t="s">
         <v>56</v>
@@ -4035,7 +4035,7 @@
         <v>34</v>
       </c>
       <c r="M51">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N51" t="s">
         <v>56</v>
@@ -4048,6 +4048,798 @@
       </c>
       <c r="Q51" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
+      <c r="A52" s="2">
+        <v>45677</v>
+      </c>
+      <c r="B52" s="2">
+        <v>45677</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="3">
+        <v>60</v>
+      </c>
+      <c r="E52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" t="s">
+        <v>20</v>
+      </c>
+      <c r="I52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" t="s">
+        <v>22</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L52" t="s">
+        <v>24</v>
+      </c>
+      <c r="M52">
+        <v>12</v>
+      </c>
+      <c r="N52" t="s">
+        <v>25</v>
+      </c>
+      <c r="O52" t="s">
+        <v>26</v>
+      </c>
+      <c r="P52" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="A53" s="2">
+        <v>45678</v>
+      </c>
+      <c r="B53" s="2">
+        <v>45678</v>
+      </c>
+      <c r="C53" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="3">
+        <v>72</v>
+      </c>
+      <c r="E53" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" t="s">
+        <v>32</v>
+      </c>
+      <c r="H53" t="s">
+        <v>20</v>
+      </c>
+      <c r="I53" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" t="s">
+        <v>22</v>
+      </c>
+      <c r="K53" t="s">
+        <v>33</v>
+      </c>
+      <c r="L53" t="s">
+        <v>34</v>
+      </c>
+      <c r="M53">
+        <v>13</v>
+      </c>
+      <c r="N53" t="s">
+        <v>35</v>
+      </c>
+      <c r="O53" t="s">
+        <v>36</v>
+      </c>
+      <c r="P53" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54" s="2">
+        <v>45679</v>
+      </c>
+      <c r="B54" s="2">
+        <v>45679</v>
+      </c>
+      <c r="C54" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="3">
+        <v>68</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" t="s">
+        <v>40</v>
+      </c>
+      <c r="G54" t="s">
+        <v>41</v>
+      </c>
+      <c r="H54" t="s">
+        <v>20</v>
+      </c>
+      <c r="I54" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" t="s">
+        <v>22</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L54" t="s">
+        <v>24</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54" t="s">
+        <v>42</v>
+      </c>
+      <c r="O54" t="s">
+        <v>43</v>
+      </c>
+      <c r="P54" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55" s="2">
+        <v>45680</v>
+      </c>
+      <c r="B55" s="2">
+        <v>45680</v>
+      </c>
+      <c r="C55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" s="3">
+        <v>75</v>
+      </c>
+      <c r="E55" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" t="s">
+        <v>40</v>
+      </c>
+      <c r="G55" t="s">
+        <v>45</v>
+      </c>
+      <c r="H55" t="s">
+        <v>46</v>
+      </c>
+      <c r="I55" t="s">
+        <v>21</v>
+      </c>
+      <c r="J55" t="s">
+        <v>22</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L55" t="s">
+        <v>24</v>
+      </c>
+      <c r="M55">
+        <v>2</v>
+      </c>
+      <c r="N55" t="s">
+        <v>48</v>
+      </c>
+      <c r="O55" t="s">
+        <v>43</v>
+      </c>
+      <c r="P55" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="A56" s="2">
+        <v>45681</v>
+      </c>
+      <c r="B56" s="2">
+        <v>45681</v>
+      </c>
+      <c r="C56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56" s="3">
+        <v>47</v>
+      </c>
+      <c r="E56" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56" t="s">
+        <v>52</v>
+      </c>
+      <c r="G56" t="s">
+        <v>53</v>
+      </c>
+      <c r="H56" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" t="s">
+        <v>22</v>
+      </c>
+      <c r="K56" t="s">
+        <v>54</v>
+      </c>
+      <c r="L56" t="s">
+        <v>55</v>
+      </c>
+      <c r="M56">
+        <v>3</v>
+      </c>
+      <c r="N56" t="s">
+        <v>56</v>
+      </c>
+      <c r="O56" t="s">
+        <v>57</v>
+      </c>
+      <c r="P56" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" s="2">
+        <v>45684</v>
+      </c>
+      <c r="B57" s="2">
+        <v>45684</v>
+      </c>
+      <c r="C57" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57" s="3">
+        <v>78</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" t="s">
+        <v>61</v>
+      </c>
+      <c r="G57" t="s">
+        <v>62</v>
+      </c>
+      <c r="H57" t="s">
+        <v>20</v>
+      </c>
+      <c r="I57" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" t="s">
+        <v>22</v>
+      </c>
+      <c r="K57" t="s">
+        <v>47</v>
+      </c>
+      <c r="L57" t="s">
+        <v>24</v>
+      </c>
+      <c r="M57">
+        <v>4</v>
+      </c>
+      <c r="N57" t="s">
+        <v>63</v>
+      </c>
+      <c r="O57" t="s">
+        <v>64</v>
+      </c>
+      <c r="P57" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58" s="2">
+        <v>45685</v>
+      </c>
+      <c r="B58" s="2">
+        <v>45685</v>
+      </c>
+      <c r="C58" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="3">
+        <v>68</v>
+      </c>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" t="s">
+        <v>67</v>
+      </c>
+      <c r="G58" t="s">
+        <v>68</v>
+      </c>
+      <c r="H58" t="s">
+        <v>46</v>
+      </c>
+      <c r="I58" t="s">
+        <v>69</v>
+      </c>
+      <c r="J58" t="s">
+        <v>22</v>
+      </c>
+      <c r="K58" t="s">
+        <v>70</v>
+      </c>
+      <c r="L58" t="s">
+        <v>34</v>
+      </c>
+      <c r="M58">
+        <v>5</v>
+      </c>
+      <c r="N58" t="s">
+        <v>71</v>
+      </c>
+      <c r="O58" t="s">
+        <v>64</v>
+      </c>
+      <c r="P58" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
+      <c r="A59" s="2">
+        <v>45686</v>
+      </c>
+      <c r="B59" s="2">
+        <v>45686</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="3">
+        <v>78</v>
+      </c>
+      <c r="E59" t="s">
+        <v>30</v>
+      </c>
+      <c r="F59" t="s">
+        <v>75</v>
+      </c>
+      <c r="G59" t="s">
+        <v>76</v>
+      </c>
+      <c r="H59" t="s">
+        <v>46</v>
+      </c>
+      <c r="I59" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" t="s">
+        <v>22</v>
+      </c>
+      <c r="K59" t="s">
+        <v>47</v>
+      </c>
+      <c r="L59" t="s">
+        <v>24</v>
+      </c>
+      <c r="M59">
+        <v>6</v>
+      </c>
+      <c r="N59" t="s">
+        <v>77</v>
+      </c>
+      <c r="O59" t="s">
+        <v>78</v>
+      </c>
+      <c r="P59" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
+      <c r="A60" s="2">
+        <v>45687</v>
+      </c>
+      <c r="B60" s="2">
+        <v>45687</v>
+      </c>
+      <c r="C60" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" s="3">
+        <v>79</v>
+      </c>
+      <c r="E60" t="s">
+        <v>30</v>
+      </c>
+      <c r="F60" t="s">
+        <v>80</v>
+      </c>
+      <c r="G60" t="s">
+        <v>81</v>
+      </c>
+      <c r="H60" t="s">
+        <v>46</v>
+      </c>
+      <c r="I60" t="s">
+        <v>69</v>
+      </c>
+      <c r="J60" t="s">
+        <v>22</v>
+      </c>
+      <c r="K60" t="s">
+        <v>82</v>
+      </c>
+      <c r="L60" t="s">
+        <v>83</v>
+      </c>
+      <c r="M60">
+        <v>7</v>
+      </c>
+      <c r="N60" t="s">
+        <v>84</v>
+      </c>
+      <c r="O60" t="s">
+        <v>78</v>
+      </c>
+      <c r="P60" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17">
+      <c r="A61" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B61" s="2">
+        <v>45688</v>
+      </c>
+      <c r="C61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" s="3">
+        <v>80</v>
+      </c>
+      <c r="E61" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" t="s">
+        <v>88</v>
+      </c>
+      <c r="G61" t="s">
+        <v>89</v>
+      </c>
+      <c r="H61" t="s">
+        <v>46</v>
+      </c>
+      <c r="I61" t="s">
+        <v>21</v>
+      </c>
+      <c r="J61" t="s">
+        <v>22</v>
+      </c>
+      <c r="K61" t="s">
+        <v>90</v>
+      </c>
+      <c r="L61" t="s">
+        <v>91</v>
+      </c>
+      <c r="M61">
+        <v>8</v>
+      </c>
+      <c r="N61" t="s">
+        <v>92</v>
+      </c>
+      <c r="O61" t="s">
+        <v>78</v>
+      </c>
+      <c r="P61" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17">
+      <c r="A62" s="2">
+        <v>45691</v>
+      </c>
+      <c r="B62" s="2">
+        <v>45691</v>
+      </c>
+      <c r="C62" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62" s="3">
+        <v>79</v>
+      </c>
+      <c r="E62" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62" t="s">
+        <v>40</v>
+      </c>
+      <c r="G62" t="s">
+        <v>96</v>
+      </c>
+      <c r="H62" t="s">
+        <v>20</v>
+      </c>
+      <c r="I62" t="s">
+        <v>21</v>
+      </c>
+      <c r="J62" t="s">
+        <v>22</v>
+      </c>
+      <c r="K62" t="s">
+        <v>90</v>
+      </c>
+      <c r="L62" t="s">
+        <v>90</v>
+      </c>
+      <c r="M62">
+        <v>9</v>
+      </c>
+      <c r="N62" t="s">
+        <v>97</v>
+      </c>
+      <c r="O62" t="s">
+        <v>78</v>
+      </c>
+      <c r="P62" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="A63" s="2">
+        <v>45692</v>
+      </c>
+      <c r="B63" s="2">
+        <v>45692</v>
+      </c>
+      <c r="C63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" s="3">
+        <v>60</v>
+      </c>
+      <c r="E63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" t="s">
+        <v>99</v>
+      </c>
+      <c r="G63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H63" t="s">
+        <v>20</v>
+      </c>
+      <c r="I63" t="s">
+        <v>21</v>
+      </c>
+      <c r="K63" t="s">
+        <v>33</v>
+      </c>
+      <c r="L63" t="s">
+        <v>34</v>
+      </c>
+      <c r="M63">
+        <v>10</v>
+      </c>
+      <c r="N63" t="s">
+        <v>71</v>
+      </c>
+      <c r="O63" t="s">
+        <v>78</v>
+      </c>
+      <c r="P63" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="A64" s="2">
+        <v>45693</v>
+      </c>
+      <c r="B64" s="2">
+        <v>45693</v>
+      </c>
+      <c r="C64" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" s="3">
+        <v>80</v>
+      </c>
+      <c r="E64" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" t="s">
+        <v>104</v>
+      </c>
+      <c r="G64" t="s">
+        <v>105</v>
+      </c>
+      <c r="H64" t="s">
+        <v>46</v>
+      </c>
+      <c r="I64" t="s">
+        <v>21</v>
+      </c>
+      <c r="J64" t="s">
+        <v>22</v>
+      </c>
+      <c r="K64" t="s">
+        <v>33</v>
+      </c>
+      <c r="L64" t="s">
+        <v>34</v>
+      </c>
+      <c r="M64">
+        <v>11</v>
+      </c>
+      <c r="N64" t="s">
+        <v>106</v>
+      </c>
+      <c r="O64" t="s">
+        <v>78</v>
+      </c>
+      <c r="P64" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="A65" s="2">
+        <v>45694</v>
+      </c>
+      <c r="B65" s="2">
+        <v>45694</v>
+      </c>
+      <c r="C65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" s="3">
+        <v>85</v>
+      </c>
+      <c r="E65" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" t="s">
+        <v>40</v>
+      </c>
+      <c r="G65" t="s">
+        <v>109</v>
+      </c>
+      <c r="H65" t="s">
+        <v>20</v>
+      </c>
+      <c r="I65" t="s">
+        <v>21</v>
+      </c>
+      <c r="J65" t="s">
+        <v>22</v>
+      </c>
+      <c r="K65" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L65" t="s">
+        <v>24</v>
+      </c>
+      <c r="M65">
+        <v>12</v>
+      </c>
+      <c r="N65" t="s">
+        <v>84</v>
+      </c>
+      <c r="O65" t="s">
+        <v>78</v>
+      </c>
+      <c r="P65" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="A66" s="2">
+        <v>45695</v>
+      </c>
+      <c r="B66" s="2">
+        <v>45695</v>
+      </c>
+      <c r="C66" t="s">
+        <v>112</v>
+      </c>
+      <c r="D66" s="3">
+        <v>69</v>
+      </c>
+      <c r="E66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" t="s">
+        <v>113</v>
+      </c>
+      <c r="H66" t="s">
+        <v>20</v>
+      </c>
+      <c r="I66" t="s">
+        <v>69</v>
+      </c>
+      <c r="J66" t="s">
+        <v>22</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L66" t="s">
+        <v>24</v>
+      </c>
+      <c r="M66">
+        <v>13</v>
+      </c>
+      <c r="N66" t="s">
+        <v>114</v>
+      </c>
+      <c r="O66" t="s">
+        <v>115</v>
+      </c>
+      <c r="P66" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>